<commit_message>
add gzip test results including pattern matching
</commit_message>
<xml_diff>
--- a/documentation/gzip/gzip.xlsx
+++ b/documentation/gzip/gzip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/gzip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3CB6FC-A970-7B4E-A20E-1B603E7233A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A255402-1632-CA47-A67B-C33E6DEBD515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52800" yWindow="-920" windowWidth="19200" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
+    <workbookView xWindow="33600" yWindow="-920" windowWidth="19200" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
   <sheets>
     <sheet name="gzip" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>QEMU</t>
   </si>
@@ -50,8 +50,32 @@
     <t>Reference Run</t>
   </si>
   <si>
+    <t>gzip Performance Testing</t>
+  </si>
+  <si>
+    <t>Workload: 500 MB testing file sourced from /dev/urandom</t>
+  </si>
+  <si>
+    <t>Native</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>gzip -k &lt;file&gt;</t>
+  </si>
+  <si>
+    <t>to Native</t>
+  </si>
+  <si>
+    <t>to QEMU</t>
+  </si>
+  <si>
     <r>
-      <t>v1.2.2-12</t>
+      <t>v1.2.2-61</t>
     </r>
     <r>
       <rPr>
@@ -61,39 +85,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (b904a345)</t>
+      <t xml:space="preserve"> (609145c0)</t>
     </r>
   </si>
   <si>
-    <t>gzip Performance Testing</t>
-  </si>
-  <si>
-    <t>Workload: 500 MB testing file sourced from /dev/urandom</t>
-  </si>
-  <si>
-    <t>Native</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>gzip -k &lt;file&gt;</t>
-  </si>
-  <si>
-    <t>to Native</t>
-  </si>
-  <si>
-    <t>to QEMU</t>
+    <r>
+      <t xml:space="preserve">v1.2.2-61 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(609145c0)</t>
+    </r>
+  </si>
+  <si>
+    <t>Versions</t>
+  </si>
+  <si>
+    <t>Post-pattern matching</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +164,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -338,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -355,109 +387,111 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -774,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2E7EA3-8BF5-F743-9E89-1A0A4F76CDF3}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E17" sqref="E17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,24 +825,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.25">
@@ -816,36 +850,36 @@
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>2</v>
@@ -853,237 +887,378 @@
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="30" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="24">
+        <v>44.405999999999999</v>
+      </c>
+      <c r="C7" s="25">
+        <v>121.622</v>
+      </c>
+      <c r="D7" s="26">
+        <f>$C7/$B7</f>
+        <v>2.7388641174616044</v>
+      </c>
+      <c r="E7" s="27">
+        <v>136.952</v>
+      </c>
+      <c r="F7" s="28">
+        <f>$E7/$B7</f>
+        <v>3.0840877358915462</v>
+      </c>
+      <c r="G7" s="29">
+        <f>$E7/$C7</f>
+        <v>1.1260462745227016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="B8" s="24">
+        <v>43.994999999999997</v>
+      </c>
+      <c r="C8" s="25">
+        <v>125.071</v>
+      </c>
+      <c r="D8" s="26">
+        <f t="shared" ref="D8:D16" si="0">$C8/$B8</f>
+        <v>2.8428457779293104</v>
+      </c>
+      <c r="E8" s="27">
+        <v>136.74700000000001</v>
+      </c>
+      <c r="F8" s="28">
+        <f t="shared" ref="F8:F16" si="1">$E8/$B8</f>
+        <v>3.108239572678714</v>
+      </c>
+      <c r="G8" s="29">
+        <f t="shared" ref="G8:G16" si="2">$E8/$C8</f>
+        <v>1.0933549743745554</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24">
+        <v>44.100999999999999</v>
+      </c>
+      <c r="C9" s="25">
+        <v>121.21899999999999</v>
+      </c>
+      <c r="D9" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7486678306614363</v>
+      </c>
+      <c r="E9" s="27">
+        <v>136.494</v>
+      </c>
+      <c r="F9" s="28">
+        <f t="shared" si="1"/>
+        <v>3.0950318586880115</v>
+      </c>
+      <c r="G9" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1260115988417658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="24">
+        <v>44.015000000000001</v>
+      </c>
+      <c r="C10" s="25">
+        <v>121.426</v>
+      </c>
+      <c r="D10" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7587413381801658</v>
+      </c>
+      <c r="E10" s="27">
+        <v>136.69499999999999</v>
+      </c>
+      <c r="F10" s="28">
+        <f t="shared" si="1"/>
+        <v>3.1056458025673064</v>
+      </c>
+      <c r="G10" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1257473687678092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24">
+        <v>44.243000000000002</v>
+      </c>
+      <c r="C11" s="25">
+        <v>121.529</v>
+      </c>
+      <c r="D11" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7468526094523424</v>
+      </c>
+      <c r="E11" s="27">
+        <v>136.518</v>
+      </c>
+      <c r="F11" s="28">
+        <f t="shared" si="1"/>
+        <v>3.0856406663200957</v>
+      </c>
+      <c r="G11" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1233368167268718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="24">
+        <v>44.545000000000002</v>
+      </c>
+      <c r="C12" s="25">
+        <v>122.09699999999999</v>
+      </c>
+      <c r="D12" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7409810304186775</v>
+      </c>
+      <c r="E12" s="27">
+        <v>137.03100000000001</v>
+      </c>
+      <c r="F12" s="28">
+        <f t="shared" si="1"/>
+        <v>3.0762375126276797</v>
+      </c>
+      <c r="G12" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1223125875328632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="24">
+        <v>44.003999999999998</v>
+      </c>
+      <c r="C13" s="25">
+        <v>121.476</v>
+      </c>
+      <c r="D13" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7605672211617125</v>
+      </c>
+      <c r="E13" s="27">
+        <v>136.99799999999999</v>
+      </c>
+      <c r="F13" s="28">
+        <f t="shared" si="1"/>
+        <v>3.1133078811017181</v>
+      </c>
+      <c r="G13" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1277783265830286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="24">
+        <v>43.771999999999998</v>
+      </c>
+      <c r="C14" s="25">
+        <v>121.414</v>
+      </c>
+      <c r="D14" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7737823266014807</v>
+      </c>
+      <c r="E14" s="27">
+        <v>136.47200000000001</v>
+      </c>
+      <c r="F14" s="28">
+        <f t="shared" si="1"/>
+        <v>3.1177921959243355</v>
+      </c>
+      <c r="G14" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1240219414565042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="24">
+        <v>44.319000000000003</v>
+      </c>
+      <c r="C15" s="25">
+        <v>121.015</v>
+      </c>
+      <c r="D15" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7305444617432704</v>
+      </c>
+      <c r="E15" s="27">
+        <v>136.51400000000001</v>
+      </c>
+      <c r="F15" s="28">
+        <f t="shared" si="1"/>
+        <v>3.0802590311153231</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1280750320208239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>10</v>
+      </c>
+      <c r="B16" s="24">
+        <v>43.968000000000004</v>
+      </c>
+      <c r="C16" s="25">
+        <v>121.417</v>
+      </c>
+      <c r="D16" s="26">
+        <f t="shared" si="0"/>
+        <v>2.7614856259097524</v>
+      </c>
+      <c r="E16" s="27">
+        <v>137.292</v>
+      </c>
+      <c r="F16" s="28">
+        <f t="shared" si="1"/>
+        <v>3.1225436681222707</v>
+      </c>
+      <c r="G16" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1307477536094617</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
-        <v>1</v>
-      </c>
-      <c r="B7" s="15">
-        <v>43.747</v>
-      </c>
-      <c r="C7" s="20">
-        <v>160.41200000000001</v>
-      </c>
-      <c r="D7" s="21">
-        <f>C7/$B7</f>
-        <v>3.6668114384986401</v>
-      </c>
-      <c r="E7" s="32">
-        <v>172.398</v>
-      </c>
-      <c r="F7" s="40">
-        <f>E7/$B7</f>
-        <v>3.9407959402930488</v>
-      </c>
-      <c r="G7" s="33">
-        <f>E7/$C7</f>
-        <v>1.0747200957534349</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
-        <v>2</v>
-      </c>
-      <c r="B8" s="15">
-        <v>43.991</v>
-      </c>
-      <c r="C8" s="20">
-        <v>161.386</v>
-      </c>
-      <c r="D8" s="21">
-        <f t="shared" ref="D8:D11" si="0">C8/$B8</f>
-        <v>3.6686140346889138</v>
-      </c>
-      <c r="E8" s="32">
-        <v>171.89699999999999</v>
-      </c>
-      <c r="F8" s="40">
-        <f t="shared" ref="F8:F11" si="1">E8/$B8</f>
-        <v>3.9075492714418858</v>
-      </c>
-      <c r="G8" s="33">
-        <f t="shared" ref="G8:G11" si="2">E8/$C8</f>
-        <v>1.0651295651419577</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
-        <v>3</v>
-      </c>
-      <c r="B9" s="15">
-        <v>44.21</v>
-      </c>
-      <c r="C9" s="20">
-        <v>161.05099999999999</v>
-      </c>
-      <c r="D9" s="21">
-        <f t="shared" si="0"/>
-        <v>3.6428636055191128</v>
-      </c>
-      <c r="E9" s="32">
-        <v>171.649</v>
-      </c>
-      <c r="F9" s="40">
-        <f t="shared" si="1"/>
-        <v>3.8825831259895951</v>
-      </c>
-      <c r="G9" s="33">
-        <f t="shared" si="2"/>
-        <v>1.0658052418178094</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
-        <v>4</v>
-      </c>
-      <c r="B10" s="15">
-        <v>43.968000000000004</v>
-      </c>
-      <c r="C10" s="20">
-        <v>161.43199999999999</v>
-      </c>
-      <c r="D10" s="21">
-        <f t="shared" si="0"/>
-        <v>3.6715793304221247</v>
-      </c>
-      <c r="E10" s="32">
-        <v>171.88</v>
-      </c>
-      <c r="F10" s="40">
-        <f t="shared" si="1"/>
-        <v>3.9092066957787477</v>
-      </c>
-      <c r="G10" s="33">
-        <f t="shared" si="2"/>
-        <v>1.0647207492938204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>5</v>
-      </c>
-      <c r="B11" s="15">
-        <v>44.040999999999997</v>
-      </c>
-      <c r="C11" s="20">
-        <v>160.47200000000001</v>
-      </c>
-      <c r="D11" s="21">
-        <f t="shared" si="0"/>
-        <v>3.6436956472378017</v>
-      </c>
-      <c r="E11" s="32">
-        <v>172.20500000000001</v>
-      </c>
-      <c r="F11" s="40">
-        <f t="shared" si="1"/>
-        <v>3.9101064916782096</v>
-      </c>
-      <c r="G11" s="33">
-        <f t="shared" si="2"/>
-        <v>1.0731155591006531</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="35"/>
-    </row>
-    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <f>AVERAGE(B7:B11)</f>
-        <v>43.991399999999999</v>
-      </c>
-      <c r="C14" s="24">
-        <f>AVERAGE(C7:C11)</f>
-        <v>160.95059999999998</v>
-      </c>
-      <c r="D14" s="44">
-        <f>AVERAGE(D7:D11)</f>
-        <v>3.6587128112733183</v>
-      </c>
-      <c r="E14" s="36">
-        <f>AVERAGE(E7:E11)</f>
-        <v>172.00579999999999</v>
-      </c>
-      <c r="F14" s="44">
-        <f>AVERAGE(F7:F11)</f>
-        <v>3.9100483050362973</v>
-      </c>
-      <c r="G14" s="25">
-        <f>AVERAGE(G7:G11)</f>
-        <v>1.0686982422215352</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <f t="shared" ref="B19:G19" si="3">AVERAGE(B7:B16)</f>
+        <v>44.136800000000008</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" si="3"/>
+        <v>121.82859999999998</v>
+      </c>
+      <c r="D19" s="21">
+        <f t="shared" si="3"/>
+        <v>2.7603332339519753</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" si="3"/>
+        <v>136.77129999999997</v>
+      </c>
+      <c r="F19" s="21">
+        <f t="shared" si="3"/>
+        <v>3.0988785925036999</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="3"/>
+        <v>1.1227432674436386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E17:G17"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>